<commit_message>
Comparing equations vs final answer
</commit_message>
<xml_diff>
--- a/v2 (extracted equations, json)/src/sympy_predict.xlsx
+++ b/v2 (extracted equations, json)/src/sympy_predict.xlsx
@@ -512,7 +512,7 @@
     <t>RandomForestClassifier</t>
   </si>
   <si>
-    <t>2023-04-13</t>
+    <t>2023-04-20</t>
   </si>
   <si>
     <t>ExtraTreesClassifier</t>
@@ -1757,16 +1757,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.824689447668171</c:v>
+                  <c:v>0.8223843625627006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8221940326818824</c:v>
+                  <c:v>0.8202709557588056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6730436230436231</c:v>
+                  <c:v>0.6697906650168549</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6779597034171503</c:v>
+                  <c:v>0.674488223916259</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1813,16 +1813,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8243473200852897</c:v>
+                  <c:v>0.8227789855072464</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.838125720598598</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6894127466086588</c:v>
+                  <c:v>0.6877283494455383</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6730515606629499</c:v>
+                  <c:v>0.6688848939962833</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1869,16 +1869,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7968627833908682</c:v>
+                  <c:v>0.7969709692838232</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8184164739355447</c:v>
+                  <c:v>0.8237562641703604</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6530483891669876</c:v>
+                  <c:v>0.6568256238476204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6219375355558083</c:v>
+                  <c:v>0.6177201236393977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1925,16 +1925,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7985656741914754</c:v>
+                  <c:v>0.7959904035058462</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7786055929171626</c:v>
+                  <c:v>0.7820468427824777</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.613905415713196</c:v>
+                  <c:v>0.6158736182148161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6439085409792543</c:v>
+                  <c:v>0.637419653354572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1981,16 +1981,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.769790558687394</c:v>
+                  <c:v>0.7688023675009836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7842443507335243</c:v>
+                  <c:v>0.7783037566741183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5929268342429784</c:v>
+                  <c:v>0.5860155195681512</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5775543482383282</c:v>
+                  <c:v>0.5773876815716615</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2037,16 +2037,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8117655468692521</c:v>
+                  <c:v>0.8102087703124756</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.8506559760490779</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6967977985950451</c:v>
+                  <c:v>0.6951326737106788</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6411719384078584</c:v>
+                  <c:v>0.6370052717411918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2093,16 +2093,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8117655468692521</c:v>
+                  <c:v>0.8102087703124756</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.8506559760490779</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6967977985950451</c:v>
+                  <c:v>0.6951326737106788</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6411719384078584</c:v>
+                  <c:v>0.6370052717411918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2149,16 +2149,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7927648232322264</c:v>
+                  <c:v>0.8047800823600799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8203465259099684</c:v>
+                  <c:v>0.8168726915015043</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6522611073137388</c:v>
+                  <c:v>0.6620395852653918</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6055059164865172</c:v>
+                  <c:v>0.6408804945575909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2205,16 +2205,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7469295565115999</c:v>
+                  <c:v>0.7458830346412794</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9111460839030446</c:v>
+                  <c:v>0.9130691608261217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5679749075692871</c:v>
+                  <c:v>0.5692874396135266</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4176881518564873</c:v>
+                  <c:v>0.4135214851898206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2986,13 +2986,13 @@
         <v>28</v>
       </c>
       <c r="B3" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>0.8190630048465266</v>
+        <v>0.817741935483871</v>
       </c>
       <c r="E3" s="2">
         <v>0.6374207188160677</v>
@@ -3001,7 +3001,7 @@
         <v>29</v>
       </c>
       <c r="G3" s="2">
-        <v>0.6772523927354277</v>
+        <v>0.6768642548372458</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3045,7 +3045,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="2">
-        <v>0.3326812803913339</v>
+        <v>0.3326541219280461</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3068,7 +3068,7 @@
         <v>35</v>
       </c>
       <c r="G6" s="2">
-        <v>0.2056139812414545</v>
+        <v>0.2056434817231029</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3091,7 +3091,7 @@
         <v>37</v>
       </c>
       <c r="G7" s="2">
-        <v>0.05242732101642594</v>
+        <v>0.05246574836558701</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3114,7 +3114,7 @@
         <v>39</v>
       </c>
       <c r="G8" s="2">
-        <v>0.2868212209899846</v>
+        <v>0.2869534940475835</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3158,7 +3158,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="2">
-        <v>0.3861254699915875</v>
+        <v>0.3860823435928762</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3181,7 +3181,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="2">
-        <v>0.274659667600017</v>
+        <v>0.274694872524393</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3204,7 +3204,7 @@
         <v>42</v>
       </c>
       <c r="G12" s="2">
-        <v>0.2072298395177741</v>
+        <v>0.2072592415739813</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3227,7 +3227,7 @@
         <v>46</v>
       </c>
       <c r="G13" s="2">
-        <v>0.2762340688310461</v>
+        <v>0.2762628448342009</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3250,7 +3250,7 @@
         <v>48</v>
       </c>
       <c r="G14" s="2">
-        <v>0.3248759668822607</v>
+        <v>0.3249044968127514</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3273,7 +3273,7 @@
         <v>48</v>
       </c>
       <c r="G15" s="2">
-        <v>0.3394035208277494</v>
+        <v>0.3394312870547767</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3296,7 +3296,7 @@
         <v>48</v>
       </c>
       <c r="G16" s="2">
-        <v>0.3192800907866939</v>
+        <v>0.3193077171311759</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3319,7 +3319,7 @@
         <v>52</v>
       </c>
       <c r="G17" s="2">
-        <v>0.3133227117498387</v>
+        <v>0.3133699521275526</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3342,7 +3342,7 @@
         <v>52</v>
       </c>
       <c r="G18" s="2">
-        <v>0.3133227117498387</v>
+        <v>0.3133699521275526</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3365,7 +3365,7 @@
         <v>52</v>
       </c>
       <c r="G19" s="2">
-        <v>0.3133227117498387</v>
+        <v>0.3133699521275526</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3388,7 +3388,7 @@
         <v>52</v>
       </c>
       <c r="G20" s="2">
-        <v>0.3133227117498387</v>
+        <v>0.3133699521275526</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3411,7 +3411,7 @@
         <v>57</v>
       </c>
       <c r="G21" s="2">
-        <v>0.5247295500620546</v>
+        <v>0.5247023869181645</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3434,7 +3434,7 @@
         <v>57</v>
       </c>
       <c r="G22" s="2">
-        <v>0.4346108579559799</v>
+        <v>0.4346805544942863</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3457,7 +3457,7 @@
         <v>60</v>
       </c>
       <c r="G23" s="2">
-        <v>0.1905575577009302</v>
+        <v>0.1905957905379247</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3480,7 +3480,7 @@
         <v>60</v>
       </c>
       <c r="G24" s="2">
-        <v>0.1330572356745862</v>
+        <v>0.1330902801447892</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3503,7 +3503,7 @@
         <v>63</v>
       </c>
       <c r="G25" s="2">
-        <v>0.1215403804755467</v>
+        <v>0.1215724432061466</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3526,7 +3526,7 @@
         <v>65</v>
       </c>
       <c r="G26" s="2">
-        <v>0.1455650687110457</v>
+        <v>0.1455987788365887</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3591,7 +3591,7 @@
         <v>69</v>
       </c>
       <c r="G29" s="2">
-        <v>0.3089929004101181</v>
+        <v>0.3090277529266906</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3614,7 +3614,7 @@
         <v>69</v>
       </c>
       <c r="G30" s="2">
-        <v>0.3089929004101181</v>
+        <v>0.3090277529266906</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -3637,7 +3637,7 @@
         <v>72</v>
       </c>
       <c r="G31" s="2">
-        <v>0.3050401656014015</v>
+        <v>0.3050779579035726</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3660,7 +3660,7 @@
         <v>72</v>
       </c>
       <c r="G32" s="2">
-        <v>0.3050401656014015</v>
+        <v>0.3050779579035726</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -3683,7 +3683,7 @@
         <v>75</v>
       </c>
       <c r="G33" s="2">
-        <v>0.1285138149495019</v>
+        <v>0.1284803972984102</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -3706,7 +3706,7 @@
         <v>75</v>
       </c>
       <c r="G34" s="2">
-        <v>0.1516947238309694</v>
+        <v>0.1517584421777476</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -3729,7 +3729,7 @@
         <v>78</v>
       </c>
       <c r="G35" s="2">
-        <v>0.1351558730984588</v>
+        <v>0.1351881339748608</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3752,7 +3752,7 @@
         <v>80</v>
       </c>
       <c r="G36" s="2">
-        <v>0.1356574254663409</v>
+        <v>0.1356904307341178</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3775,7 +3775,7 @@
         <v>82</v>
       </c>
       <c r="G37" s="2">
-        <v>0.2378858615228907</v>
+        <v>0.2379195036844709</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3798,7 +3798,7 @@
         <v>84</v>
       </c>
       <c r="G38" s="2">
-        <v>0.1495981795747803</v>
+        <v>0.1496350147007565</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3863,7 +3863,7 @@
         <v>84</v>
       </c>
       <c r="G41" s="2">
-        <v>0.2660818872291399</v>
+        <v>0.2661186297451397</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3886,7 +3886,7 @@
         <v>84</v>
       </c>
       <c r="G42" s="2">
-        <v>0.2660818872291399</v>
+        <v>0.2661186297451397</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3909,7 +3909,7 @@
         <v>84</v>
       </c>
       <c r="G43" s="2">
-        <v>0.2660818872291399</v>
+        <v>0.2661186297451397</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -3932,7 +3932,7 @@
         <v>91</v>
       </c>
       <c r="G44" s="2">
-        <v>0.3710422927261747</v>
+        <v>0.37107178107593</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3955,7 +3955,7 @@
         <v>93</v>
       </c>
       <c r="G45" s="2">
-        <v>0.1647072615881208</v>
+        <v>0.1647351932399312</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3978,7 +3978,7 @@
         <v>95</v>
       </c>
       <c r="G46" s="2">
-        <v>-0.01659905547733756</v>
+        <v>-0.01656242440981444</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -4001,7 +4001,7 @@
         <v>97</v>
       </c>
       <c r="G47" s="2">
-        <v>0.03233924282241391</v>
+        <v>0.0323762445496516</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -4087,7 +4087,7 @@
         <v>102</v>
       </c>
       <c r="G51" s="2">
-        <v>0.5033398698702825</v>
+        <v>0.5033139196761194</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -4110,7 +4110,7 @@
         <v>102</v>
       </c>
       <c r="G52" s="2">
-        <v>0.3691693990225179</v>
+        <v>0.3692044657301856</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -4133,7 +4133,7 @@
         <v>105</v>
       </c>
       <c r="G53" s="2">
-        <v>0.4081280955823248</v>
+        <v>0.4081571584504959</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -4156,7 +4156,7 @@
         <v>107</v>
       </c>
       <c r="G54" s="2">
-        <v>0.3257972691744941</v>
+        <v>0.3258243358372239</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -4179,7 +4179,7 @@
         <v>109</v>
       </c>
       <c r="G55" s="2">
-        <v>0.2136184496775336</v>
+        <v>0.2136503452774833</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -4202,7 +4202,7 @@
         <v>111</v>
       </c>
       <c r="G56" s="2">
-        <v>0.3629019195939577</v>
+        <v>0.3629360502214748</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -4225,7 +4225,7 @@
         <v>113</v>
       </c>
       <c r="G57" s="2">
-        <v>0.3644769759259929</v>
+        <v>0.3645138110519691</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -4248,7 +4248,7 @@
         <v>115</v>
       </c>
       <c r="G58" s="2">
-        <v>0.3803837904134077</v>
+        <v>0.3804278814326073</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -4271,7 +4271,7 @@
         <v>115</v>
       </c>
       <c r="G59" s="2">
-        <v>0.3803837904134077</v>
+        <v>0.3804278814326073</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -4294,7 +4294,7 @@
         <v>118</v>
       </c>
       <c r="G60" s="2">
-        <v>0.3644113338344115</v>
+        <v>0.364450280710872</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -4317,7 +4317,7 @@
         <v>118</v>
       </c>
       <c r="G61" s="2">
-        <v>0.3608603729360134</v>
+        <v>0.3608974776703102</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -4340,7 +4340,7 @@
         <v>118</v>
       </c>
       <c r="G62" s="2">
-        <v>0.3331955320531967</v>
+        <v>0.3332226355649769</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -4363,7 +4363,7 @@
         <v>122</v>
       </c>
       <c r="G63" s="2">
-        <v>0.3535599241243153</v>
+        <v>0.3535869318561117</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -4386,7 +4386,7 @@
         <v>122</v>
       </c>
       <c r="G64" s="2">
-        <v>0.374463513503524</v>
+        <v>0.3744895444119806</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -4409,7 +4409,7 @@
         <v>122</v>
       </c>
       <c r="G65" s="2">
-        <v>0.3663540884289451</v>
+        <v>0.3663800859112942</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -4432,7 +4432,7 @@
         <v>126</v>
       </c>
       <c r="G66" s="2">
-        <v>0.367342598023661</v>
+        <v>0.3673784376056918</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -4455,7 +4455,7 @@
         <v>126</v>
       </c>
       <c r="G67" s="2">
-        <v>0.367342598023661</v>
+        <v>0.3673784376056918</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -4478,7 +4478,7 @@
         <v>129</v>
       </c>
       <c r="G68" s="2">
-        <v>0.3894168516098435</v>
+        <v>0.3894624630090155</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -4501,7 +4501,7 @@
         <v>129</v>
       </c>
       <c r="G69" s="2">
-        <v>0.3894168516098435</v>
+        <v>0.3894624630090155</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -4545,7 +4545,7 @@
         <v>133</v>
       </c>
       <c r="G71" s="2">
-        <v>0.8172111107558628</v>
+        <v>0.8171882599857243</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -4568,7 +4568,7 @@
         <v>133</v>
       </c>
       <c r="G72" s="2">
-        <v>0.5752422820284095</v>
+        <v>0.5752175869433988</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -4591,7 +4591,7 @@
         <v>136</v>
       </c>
       <c r="G73" s="2">
-        <v>0.4498733152007647</v>
+        <v>0.4498301058957731</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -4614,7 +4614,7 @@
         <v>138</v>
       </c>
       <c r="G74" s="2">
-        <v>0.2626240903235862</v>
+        <v>0.2626593867560919</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -4637,7 +4637,7 @@
         <v>140</v>
       </c>
       <c r="G75" s="2">
-        <v>0.3672068013919016</v>
+        <v>0.3672382611092253</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -4660,7 +4660,7 @@
         <v>142</v>
       </c>
       <c r="G76" s="2">
-        <v>0.2652830729744534</v>
+        <v>0.2653409466471998</v>
       </c>
     </row>
   </sheetData>
@@ -7132,16 +7132,16 @@
         <v>163</v>
       </c>
       <c r="D2" s="2">
-        <v>0.824689447668171</v>
+        <v>0.8223843625627006</v>
       </c>
       <c r="E2" s="2">
-        <v>0.8221940326818824</v>
+        <v>0.8202709557588056</v>
       </c>
       <c r="F2" s="2">
-        <v>0.6730436230436231</v>
+        <v>0.6697906650168549</v>
       </c>
       <c r="G2" s="2">
-        <v>0.6779597034171503</v>
+        <v>0.674488223916259</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7152,16 +7152,16 @@
         <v>163</v>
       </c>
       <c r="D3" s="2">
-        <v>0.8243473200852897</v>
+        <v>0.8227789855072464</v>
       </c>
       <c r="E3" s="2">
         <v>0.838125720598598</v>
       </c>
       <c r="F3" s="2">
-        <v>0.6894127466086588</v>
+        <v>0.6877283494455383</v>
       </c>
       <c r="G3" s="2">
-        <v>0.6730515606629499</v>
+        <v>0.6688848939962833</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7172,16 +7172,16 @@
         <v>163</v>
       </c>
       <c r="D4" s="2">
-        <v>0.7968627833908682</v>
+        <v>0.7969709692838232</v>
       </c>
       <c r="E4" s="2">
-        <v>0.8184164739355447</v>
+        <v>0.8237562641703604</v>
       </c>
       <c r="F4" s="2">
-        <v>0.6530483891669876</v>
+        <v>0.6568256238476204</v>
       </c>
       <c r="G4" s="2">
-        <v>0.6219375355558083</v>
+        <v>0.6177201236393977</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7192,16 +7192,16 @@
         <v>163</v>
       </c>
       <c r="D5" s="2">
-        <v>0.7985656741914754</v>
+        <v>0.7959904035058462</v>
       </c>
       <c r="E5" s="2">
-        <v>0.7786055929171626</v>
+        <v>0.7820468427824777</v>
       </c>
       <c r="F5" s="2">
-        <v>0.613905415713196</v>
+        <v>0.6158736182148161</v>
       </c>
       <c r="G5" s="2">
-        <v>0.6439085409792543</v>
+        <v>0.637419653354572</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7212,16 +7212,16 @@
         <v>163</v>
       </c>
       <c r="D6" s="2">
-        <v>0.769790558687394</v>
+        <v>0.7688023675009836</v>
       </c>
       <c r="E6" s="2">
-        <v>0.7842443507335243</v>
+        <v>0.7783037566741183</v>
       </c>
       <c r="F6" s="2">
-        <v>0.5929268342429784</v>
+        <v>0.5860155195681512</v>
       </c>
       <c r="G6" s="2">
-        <v>0.5775543482383282</v>
+        <v>0.5773876815716615</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -7232,16 +7232,16 @@
         <v>163</v>
       </c>
       <c r="D7" s="2">
-        <v>0.8117655468692521</v>
+        <v>0.8102087703124756</v>
       </c>
       <c r="E7" s="2">
         <v>0.8506559760490779</v>
       </c>
       <c r="F7" s="2">
-        <v>0.6967977985950451</v>
+        <v>0.6951326737106788</v>
       </c>
       <c r="G7" s="2">
-        <v>0.6411719384078584</v>
+        <v>0.6370052717411918</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7252,16 +7252,16 @@
         <v>163</v>
       </c>
       <c r="D8" s="2">
-        <v>0.8117655468692521</v>
+        <v>0.8102087703124756</v>
       </c>
       <c r="E8" s="2">
         <v>0.8506559760490779</v>
       </c>
       <c r="F8" s="2">
-        <v>0.6967977985950451</v>
+        <v>0.6951326737106788</v>
       </c>
       <c r="G8" s="2">
-        <v>0.6411719384078584</v>
+        <v>0.6370052717411918</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7272,16 +7272,16 @@
         <v>163</v>
       </c>
       <c r="D9" s="2">
-        <v>0.7927648232322264</v>
+        <v>0.8047800823600799</v>
       </c>
       <c r="E9" s="2">
-        <v>0.8203465259099684</v>
+        <v>0.8168726915015043</v>
       </c>
       <c r="F9" s="2">
-        <v>0.6522611073137388</v>
+        <v>0.6620395852653918</v>
       </c>
       <c r="G9" s="2">
-        <v>0.6055059164865172</v>
+        <v>0.6408804945575909</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -7292,16 +7292,16 @@
         <v>163</v>
       </c>
       <c r="D10" s="2">
-        <v>0.7469295565115999</v>
+        <v>0.7458830346412794</v>
       </c>
       <c r="E10" s="2">
-        <v>0.9111460839030446</v>
+        <v>0.9130691608261217</v>
       </c>
       <c r="F10" s="2">
-        <v>0.5679749075692871</v>
+        <v>0.5692874396135266</v>
       </c>
       <c r="G10" s="2">
-        <v>0.4176881518564873</v>
+        <v>0.4135214851898206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>